<commit_message>
01June2021 selenium data driven and extent reports
</commit_message>
<xml_diff>
--- a/src/test/ressources/AutomationDemoSIte.xlsx
+++ b/src/test/ressources/AutomationDemoSIte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\seleniumMay2021\src\test\ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EF2C32-FB18-4FE4-B4FD-FA79E3412968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4337293A-B7B5-48B9-86C2-FE3A5BBF5DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestData!$A$1:$R$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,9 +44,6 @@
     <t>RunMode</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -701,7 +704,7 @@
   <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -719,450 +722,451 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>9876543210</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N2">
         <v>1987</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P2">
         <v>5</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3">
         <v>9876543211</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3">
         <v>1988</v>
       </c>
       <c r="O3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P3">
         <v>9</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4">
         <v>9876543212</v>
       </c>
       <c r="H4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N4">
         <v>1989</v>
       </c>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P4">
         <v>14</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5">
         <v>9876543213</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N5">
         <v>1990</v>
       </c>
       <c r="O5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P5">
         <v>18</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6">
         <v>9876543214</v>
       </c>
       <c r="H6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N6">
         <v>1991</v>
       </c>
       <c r="O6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P6">
         <v>21</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G7">
         <v>9876543215</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N7">
         <v>1992</v>
       </c>
       <c r="O7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P7">
         <v>27</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G8">
         <v>9876543216</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N8">
         <v>1993</v>
       </c>
       <c r="O8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P8">
         <v>30</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R8" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{BD2F6444-EE39-428E-B42C-AC019C47E23F}"/>

</xml_diff>

<commit_message>
15June2021 Selenium Page Object Repository
</commit_message>
<xml_diff>
--- a/src/test/ressources/AutomationDemoSIte.xlsx
+++ b/src/test/ressources/AutomationDemoSIte.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -389,14 +389,32 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -721,12 +739,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.796875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.6640625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.59765625" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="16.86328125" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.33203125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.59765625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.86328125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="1" spans="1:19" x14ac:dyDescent="0.45">
@@ -843,7 +861,7 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s" s="3">
+      <c r="S2" t="s" s="25">
         <v>96</v>
       </c>
     </row>
@@ -902,7 +920,7 @@
       <c r="R3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S3" t="s" s="4">
+      <c r="S3" s="19" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1017,7 +1035,7 @@
       <c r="R5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s" s="5">
+      <c r="S5" s="20" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1076,7 +1094,7 @@
       <c r="R6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S6" t="s" s="6">
+      <c r="S6" s="21" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1191,7 +1209,7 @@
       <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" t="s" s="7">
+      <c r="S8" s="22" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
16June2021 Selenium framework and testNg parameters concept and program.
</commit_message>
<xml_diff>
--- a/src/test/ressources/AutomationDemoSIte.xlsx
+++ b/src/test/ressources/AutomationDemoSIte.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -389,7 +389,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="49">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
@@ -415,6 +415,29 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -861,7 +884,7 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s" s="25">
+      <c r="S2" t="s" s="44">
         <v>96</v>
       </c>
     </row>
@@ -920,7 +943,7 @@
       <c r="R3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="S3" t="s" s="45">
         <v>96</v>
       </c>
     </row>
@@ -1035,7 +1058,7 @@
       <c r="R5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" t="s" s="46">
         <v>96</v>
       </c>
     </row>
@@ -1094,7 +1117,7 @@
       <c r="R6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S6" s="21" t="s">
+      <c r="S6" t="s" s="47">
         <v>96</v>
       </c>
     </row>
@@ -1209,7 +1232,7 @@
       <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" s="22" t="s">
+      <c r="S8" t="s" s="48">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
19June2021 included mayjune testcases testngxml file
</commit_message>
<xml_diff>
--- a/src/test/ressources/AutomationDemoSIte.xlsx
+++ b/src/test/ressources/AutomationDemoSIte.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -389,10 +389,20 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -884,7 +894,7 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s" s="44">
+      <c r="S2" t="s" s="54">
         <v>96</v>
       </c>
     </row>
@@ -943,7 +953,7 @@
       <c r="R3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S3" t="s" s="45">
+      <c r="S3" t="s" s="55">
         <v>96</v>
       </c>
     </row>
@@ -1058,7 +1068,7 @@
       <c r="R5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s" s="46">
+      <c r="S5" t="s" s="56">
         <v>96</v>
       </c>
     </row>
@@ -1117,7 +1127,7 @@
       <c r="R6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S6" t="s" s="47">
+      <c r="S6" t="s" s="57">
         <v>96</v>
       </c>
     </row>
@@ -1232,7 +1242,7 @@
       <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" t="s" s="48">
+      <c r="S8" t="s" s="58">
         <v>96</v>
       </c>
     </row>

</xml_diff>